<commit_message>
[HuyNH] Update script sql
</commit_message>
<xml_diff>
--- a/01.Database/02.Document/DATABASE_TABLE_SCHEMA_SYS.xlsx
+++ b/01.Database/02.Document/DATABASE_TABLE_SCHEMA_SYS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study8-parent\study8-document\01.Database\02.Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D67FB9-1D10-4348-A886-9FBD4A31BE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1453F3BF-6CDA-42D9-B557-610973B6EA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1F8EE15-CA5F-4E45-ACBA-B39BFBE9925C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A1F8EE15-CA5F-4E45-ACBA-B39BFBE9925C}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Of Content" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
-  <si>
-    <t>STT</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -207,6 +204,21 @@
       <t>. This is an internal document, please do not share it. 
 STUDY8, from Ho Chi Minh City, Vietnam 🐉</t>
     </r>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Length</t>
   </si>
 </sst>
 </file>
@@ -295,7 +307,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +317,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -392,6 +410,22 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -722,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4ADDC14-CB05-4FA2-97B6-3CDD84CCD240}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,31 +773,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="A1" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>1</v>
-      </c>
       <c r="C4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -772,10 +806,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="8"/>
     </row>
@@ -784,10 +818,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="8"/>
     </row>
@@ -796,42 +830,42 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="C11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="F11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="16" t="s">
         <v>5</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -839,21 +873,21 @@
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="5">
         <v>45526.462500000001</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="14"/>
       <c r="H12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -861,21 +895,21 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5">
         <v>45527.462500000001</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="15"/>
       <c r="H13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -883,21 +917,21 @@
         <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5">
         <v>45528.462500000001</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="15"/>
       <c r="H14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -905,21 +939,21 @@
         <v>4</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5">
         <v>45529.462500000001</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="15"/>
       <c r="H15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -927,44 +961,44 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="5">
         <v>45530.462500000001</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="15"/>
       <c r="H16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="A19" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -986,12 +1020,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2097D109-F2FE-45A2-8660-9F4CDE14C99D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="24" t="str">
+        <f>'Table Of Content'!B12</f>
+        <v>app_role</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="21" t="str">
+        <f>'Table Of Content'!C12</f>
+        <v>List of system role</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="22">
+        <f>'Table Of Content'!D12</f>
+        <v>45526.462500000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23" t="str">
+        <f>'Table Of Content'!E12</f>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21" t="str">
+        <f>'Table Of Content'!H12</f>
+        <v>HuyNH</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>